<commit_message>
update  WA country code
</commit_message>
<xml_diff>
--- a/TestData/User_Import.xlsx
+++ b/TestData/User_Import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CFLOW PLAYWRIGHT\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3585D7E2-428C-4F30-ACD9-938CD6ED7487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A517765F-1EAB-4A6C-AE9E-F0F011311C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,13 +52,13 @@
     <t>importuser01@yopmail.com</t>
   </si>
   <si>
-    <t>import user 4</t>
-  </si>
-  <si>
-    <t>importuser04</t>
-  </si>
-  <si>
-    <t>IM43</t>
+    <t>import user 6</t>
+  </si>
+  <si>
+    <t>importuser06</t>
+  </si>
+  <si>
+    <t>IM45</t>
   </si>
 </sst>
 </file>
@@ -939,7 +939,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>9994397458</v>
+        <v>9994397460</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -1002,7 +1002,7 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{30ED8197-E0E1-4D0D-AAB5-DB52A3775A39}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{5C29D571-B0F8-4D9A-AA40-141C7C468A71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>